<commit_message>
Stage 2 and stage 3
</commit_message>
<xml_diff>
--- a/kadiralan/evidence.xlsx
+++ b/kadiralan/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kadiralan/Desktop/Testnet/Projects/gon-evidence/kadiralan/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA27FDDD-11D0-E840-B470-DA2E58269236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC727FF-B7C7-294A-AAC3-7611CFFC35D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" firstSheet="10" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -38,47 +38,30 @@
     <sheet name="B2" sheetId="23" r:id="rId23"/>
     <sheet name="B5" sheetId="24" r:id="rId24"/>
     <sheet name="B6" sheetId="25" r:id="rId25"/>
+    <sheet name="B7" sheetId="27" r:id="rId26"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="95">
   <si>
     <t>TxHash</t>
   </si>
   <si>
-    <t>The first Interchain NFT-Transfer TxHash</t>
-  </si>
-  <si>
     <t>The Internal Transfer TxHash on IRISnet</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>9FAA9F48785F6379F0A36C6590CF5607F07969EFC5E1A107B09533719D8BB932</t>
   </si>
   <si>
@@ -167,13 +150,193 @@
   </si>
   <si>
     <t>none</t>
+  </si>
+  <si>
+    <t>nft07</t>
+  </si>
+  <si>
+    <t>ibc/851D6590690A792C4E6A5B4BF144937AE7EBB85F993B015D7671FCE4F3E9AFD9</t>
+  </si>
+  <si>
+    <t>nft08</t>
+  </si>
+  <si>
+    <t>ibc/5235EAE9F603EB05576998363DA7AB5DDE016DA0B84B77BA7196DDF982D673D2</t>
+  </si>
+  <si>
+    <t>nft09</t>
+  </si>
+  <si>
+    <t>ibc/EC308A2A6725EB7060A88DA8731EB5947AA4B5FABBD6213B3F1F1E9843DAE718</t>
+  </si>
+  <si>
+    <t>nft10</t>
+  </si>
+  <si>
+    <t>ibc/46118A87905CD060C9F8B8C1055384C8D52BE12EA9270AB3C6241D4C4EDD8E7E</t>
+  </si>
+  <si>
+    <t>nft11</t>
+  </si>
+  <si>
+    <t>ibc/3239F0522A2808EB5C96658A36987037EB67BCB608365A458735896153E4FC06</t>
+  </si>
+  <si>
+    <t>nft12</t>
+  </si>
+  <si>
+    <t>ibc/57945F6D4FD66E8730471E7CDD302DB1145449802003858AEDE45E29F9F68C57</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>5337B1E90AEC3D9C69DA4E7C4CF409D7243F67CCB8921D891336BE42DAEB6C8F</t>
+  </si>
+  <si>
+    <t>212F27553ABF67DA34CB711BB0AAEB15EBCE6A3844AEB39363736FCEF295BF6F</t>
+  </si>
+  <si>
+    <t>599CC95A7ECC42B472083E731CD4E632F22985E59F8376DC902E5ADBFF34CB44</t>
+  </si>
+  <si>
+    <t>94C8C3639D3D6DE5B8812342DFE1F7542CE88568DFFFA25F9ECA08BF69B1A715</t>
+  </si>
+  <si>
+    <t>96A0C89B30C5976DE4C963601C381650E9FF3B49E8A9F4350076CE6C13B36CFC</t>
+  </si>
+  <si>
+    <t>11327C1EA26FF7252E7ECD7199E0E398DD8A0803E53E73275D04CA402C7F62E2</t>
+  </si>
+  <si>
+    <t>29FD6A72D08DFAA8E0BB82380DEC4A7662E8043A594BF2A03DBA0C75357BC784</t>
+  </si>
+  <si>
+    <t>227A244DB3F9514965FF85308FE3A873BEEE8AB35801639B83064FA05751B156</t>
+  </si>
+  <si>
+    <t>ADB98F83E547A6456ED9A8E0A9A0D158CB4E4685A0F04F692AE7ACEE733B6776</t>
+  </si>
+  <si>
+    <t>44C36E845D27B4936C6CEA4450636C262F36E60231F42CA8E1AF87237D8AA79D</t>
+  </si>
+  <si>
+    <t>CB56089427D3080D04DE59557D191CE3F1ECD9805C0279957770F47D6150E0DA</t>
+  </si>
+  <si>
+    <t>96EEC93D9AD447EAFC9E49FEB6D5B3BC2DD30FCD44AF86E6A5E72415529638C9</t>
+  </si>
+  <si>
+    <t>EC0C833FA01E4181BDF025E90615A9183E6C89170C87AC2FC172F774A538DD64</t>
+  </si>
+  <si>
+    <t>E1338AE509BDADA3781E3F0C07FE242D617A668834D7065CDB18D1B097CFD493</t>
+  </si>
+  <si>
+    <t>25222C5A721E541B3DEFBC853178E7A281EB370B718D3EC232C26B493EE30652</t>
+  </si>
+  <si>
+    <t>9A0175E47B5817FFB4885EB82D782EBCBE6992FC6998B951DDC50CA612E6FF99</t>
+  </si>
+  <si>
+    <t>2ADE44243DA8063CC1D2A40114243F3648BCE9F0BDE167E124D55BE11573E773</t>
+  </si>
+  <si>
+    <t>081C3C12A40FEF0D1AA436C8D89B77CF215E19B3F07E0860E5BB3093DABE4A15</t>
+  </si>
+  <si>
+    <t>8FF6166118B535211371EB8D36F3FD44D918E249282B2039B1603132B7AAC72D</t>
+  </si>
+  <si>
+    <t>5E747DC3A009D2C607F26786EFA565D3B73F759A53A7BFB3857EB85EFC8BAA97</t>
+  </si>
+  <si>
+    <t>CAB3E0AAB11249396844275BC4264D1942737FE8C7EA18DA306C3BFA6B925B67</t>
+  </si>
+  <si>
+    <t>4EF25A3E09FD1184CE9648D36E37AB7342E2959637D4E0F0F9814B2DE5E47D67</t>
+  </si>
+  <si>
+    <t>C9279C0E37E357B798AA4809E8FD1260AD6E26B42DE0040C97FC29709F8F916D</t>
+  </si>
+  <si>
+    <t>3E67B75FF03D4F17DA803323771148498FB80B857BEAF9B7E89CC657843D2402</t>
+  </si>
+  <si>
+    <t>7C929E44A0D8B6D94E0ACB34F8E6B08B19723F8D1FA624C2389E91F6F2F7D91A</t>
+  </si>
+  <si>
+    <t>9127F391A6407F500B23D710B547A6BC392D366C22B2E91E20AC30385E505597</t>
+  </si>
+  <si>
+    <t>B6FEA79857EF74177C4744950FB2680C367A5758CCB0250096D9A440D20AF96C</t>
+  </si>
+  <si>
+    <t>74C8C26661CEEEC90E6250C558DFFA411E9CD0664ED7E8A321E7B760A4EFA836</t>
+  </si>
+  <si>
+    <t>161BD0CEED6EC5D7EE1149946D7473261844B14D6AE7EA63CC89EA30AE8812F5</t>
+  </si>
+  <si>
+    <t>B360C334E9BF80404819FFA00D67935BEF25A54DD67CD77481D09AB057CBE40E</t>
+  </si>
+  <si>
+    <t>DD3D768F2D2F5F08F8B380DE3A4726FFBEBAD00EEEE28192C9CB111628D612A9</t>
+  </si>
+  <si>
+    <t>3824CCAD043DFFAF83DC9049B770AF8A8595741480F2AEFFBA50696CD4F78059</t>
+  </si>
+  <si>
+    <t>0E9C4A6BDD684697992A4045C4C839738A1F11665C12F02E6F80A25C88C3CC7F</t>
+  </si>
+  <si>
+    <t>E00C9BF0B422580C3FF2ACF9CCB6F755B92C1D64663BEFE0F9061671CFF5D9F1</t>
+  </si>
+  <si>
+    <t>27A8D8D40D84760E9EAFA5B6E64FB74AF15F54E6FF93F8F7C5D5D6FEC98AACEF</t>
+  </si>
+  <si>
+    <t>96AF7FB44B2926C6F99D900C487601946F72D56034522E38B99E84911989BABD</t>
+  </si>
+  <si>
+    <t>CE5791B773B8D1A9F1998A0900318660A7EB2CC6226FA621923786F1E3DA575D</t>
+  </si>
+  <si>
+    <t>F1CD6E75FC6B9A3F7BAA14C615DBB6CAB3632A7064F75DFF363CEB7CD7032C3E</t>
+  </si>
+  <si>
+    <t>5C8D22D40D590DEA84F8EA12F98FF5E07464327E628A6D88E73668EA6CE2553A</t>
+  </si>
+  <si>
+    <t>4ACD0D66CDB7271A08A78232D6A99CA93B6ADE4B73963EFEE18751D083A33888</t>
+  </si>
+  <si>
+    <t>9E06691A2CF29EF7A57272B819DC5C6313F9629A5C1C710A7DED89B9733F570B</t>
+  </si>
+  <si>
+    <t>08EB379CF9E837CEC7BBCCB9E620FE0F96FB824CF2632E5BB5CE6ABEB40D94F0</t>
+  </si>
+  <si>
+    <t>3E8032768A9F8951C2865CFBD1E4E3827F5FBB70B003CB9D5C308AADA0012B83</t>
+  </si>
+  <si>
+    <t>C4DAE5D251EE8B6879A12E5AF5744085929B39A6F5B740F98FB844FF3E96D428</t>
+  </si>
+  <si>
+    <t>DA2406AC47DB02618A041C9490C966147765CE79C489E846DC7D781F6789602B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +355,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -246,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -264,6 +434,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,54 +766,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="H2" t="s">
         <v>34</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -651,7 +828,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -661,18 +840,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +866,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -697,18 +878,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -723,7 +904,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -733,18 +916,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -759,7 +942,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -769,18 +954,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -793,14 +978,388 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="232" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="213" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="119" zoomScaleNormal="119" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="171" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="218" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView zoomScale="207" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -813,39 +1372,109 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="246" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+        <v>76</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView zoomScale="286" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -854,338 +1483,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>81</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="17.83203125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>82</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1200,11 +1546,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1214,12 +1562,12 @@
     </row>
     <row r="2" spans="1:1" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1234,11 +1582,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1248,12 +1598,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1268,11 +1618,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1282,12 +1634,12 @@
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1302,11 +1654,13 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1315,13 +1669,49 @@
       </c>
     </row>
     <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="9" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8376EAAE-8756-D945-BCE1-009EF85C128B}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="72.1640625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1336,7 +1726,7 @@
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -1352,32 +1742,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -1408,27 +1798,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1460,27 +1850,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1509,27 +1899,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1561,27 +1951,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1596,7 +1986,47 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="74.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1606,54 +2036,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>